<commit_message>
Big catch up. Updated final code, added Variability_Functions.R, removal_analysis.R, etc.
</commit_message>
<xml_diff>
--- a/Variability Table.xlsx
+++ b/Variability Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jesse/Documents/GitHub/EEID_1A_Mechanistic_Link/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DBE981DA-AC85-864B-8A51-A1A21ED08083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E3FBBD0-593D-7D45-A0A9-87E79E056026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42860" yWindow="1680" windowWidth="27640" windowHeight="16440" activeTab="1" xr2:uid="{E9341F8B-2029-3449-939C-14AB189A6391}"/>
+    <workbookView xWindow="5200" yWindow="1840" windowWidth="27640" windowHeight="16440" activeTab="1" xr2:uid="{E9341F8B-2029-3449-939C-14AB189A6391}"/>
   </bookViews>
   <sheets>
     <sheet name="Variability Table" sheetId="1" r:id="rId1"/>
@@ -722,15 +722,6 @@
   </cellStyleXfs>
   <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -739,21 +730,12 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -762,51 +744,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -832,27 +784,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -874,18 +805,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -897,9 +819,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -914,32 +833,113 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1357,479 +1357,479 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="90" t="s">
+      <c r="B1" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
     </row>
     <row r="2" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="3"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="63"/>
     </row>
     <row r="3" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="6">
         <v>5.0912899999999997E-2</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="6">
         <v>7.3105160000000002E-2</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="7">
         <v>6.3386410000000004E-2</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B5" s="12"/>
-      <c r="C5" s="13" t="s">
+      <c r="B5" s="65"/>
+      <c r="C5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="9">
         <v>5.3414650000000001E-2</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="9">
         <v>7.2896870000000002E-2</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="10">
         <v>6.3187080000000007E-2</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B6" s="12"/>
-      <c r="C6" s="9" t="s">
+      <c r="B6" s="65"/>
+      <c r="C6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="6">
         <v>5.3414650000000001E-2</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="6">
         <v>7.2896870000000002E-2</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="7">
         <v>6.3187080000000007E-2</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B7" s="12"/>
-      <c r="C7" s="13" t="s">
+      <c r="B7" s="65"/>
+      <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="9">
         <v>2.8450073999999998E-3</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="9">
         <v>5.2858647000000002E-3</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="10">
         <v>3.9767301E-3</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B8" s="12"/>
-      <c r="C8" s="9" t="s">
+      <c r="B8" s="65"/>
+      <c r="C8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="6">
         <v>5.3338610000000002E-2</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="6">
         <v>7.2703950000000003E-2</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="7">
         <v>6.3061320000000004E-2</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B9" s="16"/>
-      <c r="C9" s="13" t="s">
+      <c r="B9" s="66"/>
+      <c r="C9" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9" s="9">
         <v>2.661558E-2</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="9">
         <v>3.890354E-2</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="10">
         <v>3.3435470000000002E-2</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="19">
+      <c r="D10" s="13">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="E10" s="19">
+      <c r="E10" s="13">
         <v>4.7E-2</v>
       </c>
-      <c r="F10" s="20">
+      <c r="F10" s="14">
         <v>4.6199999999999998E-2</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="23">
+      <c r="D11" s="17">
         <v>46</v>
       </c>
-      <c r="E11" s="23">
+      <c r="E11" s="17">
         <v>51</v>
       </c>
-      <c r="F11" s="24">
+      <c r="F11" s="18">
         <v>53</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="26"/>
+      <c r="C12" s="62"/>
+      <c r="D12" s="67"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="68"/>
     </row>
     <row r="13" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="6">
         <v>3.2535090000000003E-2</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="6">
         <v>0.26451003000000001</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F14" s="7">
         <v>0.26597706999999998</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B15" s="12"/>
-      <c r="C15" s="13" t="s">
+      <c r="B15" s="65"/>
+      <c r="C15" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15" s="9">
         <v>3.0250800000000001E-2</v>
       </c>
-      <c r="E15" s="14">
+      <c r="E15" s="9">
         <v>0.41415729000000001</v>
       </c>
-      <c r="F15" s="15">
+      <c r="F15" s="10">
         <v>0.32466658999999998</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B16" s="12"/>
-      <c r="C16" s="9" t="s">
+      <c r="B16" s="65"/>
+      <c r="C16" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="6">
         <v>3.0250800000000001E-2</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16" s="6">
         <v>0.34537245</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="7">
         <v>0.30228899999999997</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B17" s="12"/>
-      <c r="C17" s="13" t="s">
+      <c r="B17" s="65"/>
+      <c r="C17" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="14">
+      <c r="D17" s="9">
         <v>9.1427429999999996E-4</v>
       </c>
-      <c r="E17" s="14">
+      <c r="E17" s="9">
         <v>0.1464126496</v>
       </c>
-      <c r="F17" s="15">
+      <c r="F17" s="10">
         <v>9.5356972200000001E-2</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B18" s="12"/>
-      <c r="C18" s="9" t="s">
+      <c r="B18" s="65"/>
+      <c r="C18" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D18" s="6">
         <v>3.0236969999999998E-2</v>
       </c>
-      <c r="E18" s="10">
+      <c r="E18" s="6">
         <v>0.32645091999999998</v>
       </c>
-      <c r="F18" s="11">
+      <c r="F18" s="7">
         <v>0.28935741999999998</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B19" s="16"/>
-      <c r="C19" s="13" t="s">
+      <c r="B19" s="66"/>
+      <c r="C19" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="14">
+      <c r="D19" s="9">
         <v>1.6276499999999999E-2</v>
       </c>
-      <c r="E19" s="14">
+      <c r="E19" s="9">
         <v>0.1917585</v>
       </c>
-      <c r="F19" s="15">
+      <c r="F19" s="10">
         <v>0.172289</v>
       </c>
     </row>
     <row r="20" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="27">
+      <c r="D20" s="19">
         <v>4.4200000000000003E-2</v>
       </c>
-      <c r="E20" s="27">
+      <c r="E20" s="19">
         <v>6.93E-2</v>
       </c>
-      <c r="F20" s="28">
+      <c r="F20" s="20">
         <v>9.5299999999999996E-2</v>
       </c>
     </row>
     <row r="21" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="21" t="s">
+      <c r="B21" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="22" t="s">
+      <c r="C21" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="23">
+      <c r="D21" s="17">
         <v>32</v>
       </c>
-      <c r="E21" s="23">
+      <c r="E21" s="17">
         <v>50</v>
       </c>
-      <c r="F21" s="24">
+      <c r="F21" s="18">
         <v>53</v>
       </c>
     </row>
     <row r="22" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="26"/>
+      <c r="C22" s="62"/>
+      <c r="D22" s="67"/>
+      <c r="E22" s="67"/>
+      <c r="F22" s="68"/>
     </row>
     <row r="23" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="E23" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="F23" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D24" s="10">
+      <c r="D24" s="6">
         <v>5.9173539999999997E-2</v>
       </c>
-      <c r="E24" s="10">
+      <c r="E24" s="6">
         <v>0.12567798999999999</v>
       </c>
-      <c r="F24" s="11">
+      <c r="F24" s="7">
         <v>0.18708483000000001</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B25" s="12"/>
-      <c r="C25" s="13" t="s">
+      <c r="B25" s="65"/>
+      <c r="C25" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D25" s="14">
+      <c r="D25" s="9">
         <v>7.1008539999999995E-2</v>
       </c>
-      <c r="E25" s="14">
+      <c r="E25" s="9">
         <v>0.15269055000000001</v>
       </c>
-      <c r="F25" s="15">
+      <c r="F25" s="10">
         <v>0.26056457999999999</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B26" s="12"/>
-      <c r="C26" s="9" t="s">
+      <c r="B26" s="65"/>
+      <c r="C26" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D26" s="10">
+      <c r="D26" s="6">
         <v>7.100853E-2</v>
       </c>
-      <c r="E26" s="10">
+      <c r="E26" s="6">
         <v>0.14085871</v>
       </c>
-      <c r="F26" s="11">
+      <c r="F26" s="7">
         <v>0.22625635999999999</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B27" s="12"/>
-      <c r="C27" s="13" t="s">
+      <c r="B27" s="65"/>
+      <c r="C27" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D27" s="14">
+      <c r="D27" s="9">
         <v>5.0169157999999997E-3</v>
       </c>
-      <c r="E27" s="14">
+      <c r="E27" s="9">
         <v>2.27832273E-2</v>
       </c>
-      <c r="F27" s="15">
+      <c r="F27" s="10">
         <v>6.35773855E-2</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B28" s="12"/>
-      <c r="C28" s="9" t="s">
+      <c r="B28" s="65"/>
+      <c r="C28" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D28" s="10">
+      <c r="D28" s="6">
         <v>7.0830190000000001E-2</v>
       </c>
-      <c r="E28" s="10">
+      <c r="E28" s="6">
         <v>0.13948177</v>
       </c>
-      <c r="F28" s="11">
+      <c r="F28" s="7">
         <v>0.22067837000000001</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B29" s="16"/>
-      <c r="C29" s="13" t="s">
+      <c r="B29" s="66"/>
+      <c r="C29" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D29" s="14">
+      <c r="D29" s="9">
         <v>3.2058139999999999E-2</v>
       </c>
-      <c r="E29" s="14">
+      <c r="E29" s="9">
         <v>7.4280959999999993E-2</v>
       </c>
-      <c r="F29" s="15">
+      <c r="F29" s="10">
         <v>0.12140402</v>
       </c>
     </row>
     <row r="30" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="17" t="s">
+      <c r="B30" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="18" t="s">
+      <c r="C30" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D30" s="27">
+      <c r="D30" s="19">
         <v>4.4400000000000002E-2</v>
       </c>
-      <c r="E30" s="27">
+      <c r="E30" s="19">
         <v>4.9799999999999997E-2</v>
       </c>
-      <c r="F30" s="28">
+      <c r="F30" s="20">
         <v>5.7799999999999997E-2</v>
       </c>
     </row>
     <row r="31" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="21" t="s">
+      <c r="B31" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C31" s="22" t="s">
+      <c r="C31" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D31" s="23">
+      <c r="D31" s="17">
         <v>46</v>
       </c>
-      <c r="E31" s="29">
+      <c r="E31" s="21">
         <v>50</v>
       </c>
-      <c r="F31" s="24">
+      <c r="F31" s="18">
         <v>53</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B24:B29"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B4:B9"/>
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="B14:B19"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B24:B29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1840,7 +1840,7 @@
   <dimension ref="B1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1855,418 +1855,428 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="30" t="s">
+      <c r="H1" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="30" t="s">
+      <c r="I1" s="22" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="2:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="86" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="88" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="33" t="s">
+      <c r="D2" s="85" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="34" t="s">
+      <c r="E2" s="79" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="34" t="s">
+      <c r="F2" s="79" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="35" t="s">
+      <c r="G2" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="35" t="s">
+      <c r="H2" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="34" t="s">
+      <c r="I2" s="79" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="B3" s="31"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37" t="s">
+    <row r="3" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B3" s="86"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="38" t="s">
+      <c r="H3" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="I3" s="37"/>
+      <c r="I3" s="72"/>
     </row>
     <row r="4" spans="2:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="B4" s="31"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37" t="s">
+      <c r="B4" s="86"/>
+      <c r="C4" s="89"/>
+      <c r="D4" s="85"/>
+      <c r="E4" s="72"/>
+      <c r="F4" s="72" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="37"/>
-      <c r="H4" s="38" t="s">
+      <c r="G4" s="72"/>
+      <c r="H4" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="I4" s="37"/>
-    </row>
-    <row r="5" spans="2:9" ht="68" x14ac:dyDescent="0.2">
-      <c r="B5" s="31"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="40" t="s">
+      <c r="I4" s="72"/>
+    </row>
+    <row r="5" spans="2:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="B5" s="86"/>
+      <c r="C5" s="90"/>
+      <c r="D5" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="41"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="38" t="s">
+      <c r="E5" s="91"/>
+      <c r="F5" s="72"/>
+      <c r="G5" s="72"/>
+      <c r="H5" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="I5" s="37"/>
+      <c r="I5" s="72"/>
     </row>
     <row r="6" spans="2:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="B6" s="42"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="43" t="s">
+      <c r="B6" s="87"/>
+      <c r="C6" s="90"/>
+      <c r="D6" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="E6" s="41"/>
-      <c r="F6" s="44" t="s">
+      <c r="E6" s="91"/>
+      <c r="F6" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="G6" s="37"/>
-      <c r="H6" s="38" t="s">
+      <c r="G6" s="72"/>
+      <c r="H6" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="I6" s="37"/>
+      <c r="I6" s="72"/>
     </row>
     <row r="7" spans="2:9" ht="69" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="46" t="s">
+      <c r="C7" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="47" t="s">
+      <c r="D7" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="48" t="s">
+      <c r="E7" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="49" t="s">
+      <c r="F7" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="G7" s="50" t="s">
+      <c r="G7" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="H7" s="51" t="s">
+      <c r="H7" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="I7" s="52"/>
+      <c r="I7" s="36"/>
     </row>
     <row r="8" spans="2:9" ht="68" x14ac:dyDescent="0.2">
-      <c r="B8" s="53" t="s">
+      <c r="B8" s="69" t="s">
         <v>51</v>
       </c>
-      <c r="C8" s="37" t="s">
+      <c r="C8" s="72" t="s">
         <v>52</v>
       </c>
-      <c r="D8" s="54" t="s">
+      <c r="D8" s="83" t="s">
         <v>53</v>
       </c>
-      <c r="E8" s="55" t="s">
+      <c r="E8" s="74" t="s">
         <v>54</v>
       </c>
-      <c r="F8" s="37" t="s">
+      <c r="F8" s="72" t="s">
         <v>55</v>
       </c>
-      <c r="G8" s="38" t="s">
+      <c r="G8" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="H8" s="38" t="s">
+      <c r="H8" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="I8" s="38" t="s">
+      <c r="I8" s="24" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="B9" s="56"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="38" t="s">
+      <c r="B9" s="70"/>
+      <c r="C9" s="72"/>
+      <c r="D9" s="85"/>
+      <c r="E9" s="74"/>
+      <c r="F9" s="72"/>
+      <c r="G9" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="H9" s="38" t="s">
+      <c r="H9" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="I9" s="38" t="s">
+      <c r="I9" s="24" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="10" spans="2:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="B10" s="56"/>
-      <c r="C10" s="57" t="s">
+      <c r="B10" s="70"/>
+      <c r="C10" s="80" t="s">
         <v>62</v>
       </c>
-      <c r="D10" s="40" t="s">
+      <c r="D10" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="E10" s="58"/>
-      <c r="F10" s="37" t="s">
+      <c r="E10" s="82"/>
+      <c r="F10" s="72" t="s">
         <v>64</v>
       </c>
-      <c r="G10" s="38" t="s">
+      <c r="G10" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="H10" s="38" t="s">
+      <c r="H10" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="I10" s="38" t="s">
+      <c r="I10" s="24" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="11" spans="2:9" ht="68" x14ac:dyDescent="0.2">
-      <c r="B11" s="59"/>
-      <c r="C11" s="57"/>
-      <c r="D11" s="43" t="s">
+      <c r="B11" s="84"/>
+      <c r="C11" s="80"/>
+      <c r="D11" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="E11" s="58"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="60" t="s">
+      <c r="E11" s="82"/>
+      <c r="F11" s="72"/>
+      <c r="G11" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="H11" s="60" t="s">
+      <c r="H11" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="I11" s="60" t="s">
+      <c r="I11" s="37" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="12" spans="2:9" ht="69" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="61" t="s">
+      <c r="B12" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="61" t="s">
+      <c r="C12" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="62" t="s">
+      <c r="D12" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="E12" s="63" t="s">
+      <c r="E12" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="F12" s="49" t="s">
+      <c r="F12" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="G12" s="91" t="s">
+      <c r="G12" s="59" t="s">
         <v>49</v>
       </c>
-      <c r="H12" s="65"/>
-      <c r="I12" s="66"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="43"/>
     </row>
     <row r="13" spans="2:9" ht="68" x14ac:dyDescent="0.2">
-      <c r="B13" s="69" t="s">
+      <c r="B13" s="76" t="s">
         <v>72</v>
       </c>
-      <c r="C13" s="34" t="s">
+      <c r="C13" s="79" t="s">
         <v>73</v>
       </c>
-      <c r="D13" s="70" t="e" vm="1">
+      <c r="D13" s="46" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="E13" s="71" t="s">
+      <c r="E13" s="81" t="s">
         <v>54</v>
       </c>
-      <c r="F13" s="35" t="s">
+      <c r="F13" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="G13" s="68" t="s">
+      <c r="G13" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="H13" s="35" t="s">
+      <c r="H13" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="I13" s="35" t="s">
+      <c r="I13" s="23" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="68" x14ac:dyDescent="0.2">
-      <c r="B14" s="72"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="73" t="s">
+      <c r="B14" s="77"/>
+      <c r="C14" s="80"/>
+      <c r="D14" s="47" t="s">
         <v>78</v>
       </c>
-      <c r="E14" s="58"/>
-      <c r="F14" s="37" t="s">
+      <c r="E14" s="82"/>
+      <c r="F14" s="72" t="s">
         <v>79</v>
       </c>
-      <c r="G14" s="74" t="s">
+      <c r="G14" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="H14" s="75" t="s">
+      <c r="H14" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="I14" s="37" t="s">
+      <c r="I14" s="72" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="15" spans="2:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="B15" s="72"/>
-      <c r="C15" s="57"/>
-      <c r="D15" s="76" t="s">
+      <c r="B15" s="77"/>
+      <c r="C15" s="80"/>
+      <c r="D15" s="50" t="s">
         <v>82</v>
       </c>
-      <c r="E15" s="58"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="55" t="s">
+      <c r="E15" s="82"/>
+      <c r="F15" s="72"/>
+      <c r="G15" s="74" t="s">
         <v>83</v>
       </c>
-      <c r="H15" s="37" t="s">
+      <c r="H15" s="72" t="s">
         <v>84</v>
       </c>
-      <c r="I15" s="37"/>
+      <c r="I15" s="72"/>
     </row>
     <row r="16" spans="2:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="B16" s="77"/>
-      <c r="C16" s="57"/>
-      <c r="D16" s="67" t="s">
+      <c r="B16" s="78"/>
+      <c r="C16" s="80"/>
+      <c r="D16" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="E16" s="58"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="55"/>
-      <c r="H16" s="54"/>
-      <c r="I16" s="54"/>
+      <c r="E16" s="82"/>
+      <c r="F16" s="72"/>
+      <c r="G16" s="74"/>
+      <c r="H16" s="83"/>
+      <c r="I16" s="83"/>
     </row>
     <row r="17" spans="2:9" ht="69" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="78" t="s">
+      <c r="B17" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="79" t="s">
+      <c r="C17" s="52" t="s">
         <v>86</v>
       </c>
-      <c r="D17" s="80" t="s">
+      <c r="D17" s="53" t="s">
         <v>87</v>
       </c>
-      <c r="E17" s="63" t="s">
+      <c r="E17" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="F17" s="49" t="s">
+      <c r="F17" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="G17" s="81" t="s">
+      <c r="G17" s="54" t="s">
         <v>88</v>
       </c>
-      <c r="H17" s="64"/>
-      <c r="I17" s="66"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="43"/>
     </row>
     <row r="18" spans="2:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="B18" s="53" t="s">
+      <c r="B18" s="69" t="s">
         <v>89</v>
       </c>
-      <c r="C18" s="37" t="s">
+      <c r="C18" s="72" t="s">
         <v>90</v>
       </c>
-      <c r="D18" s="74" t="e" vm="2">
+      <c r="D18" s="48" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
-      <c r="E18" s="55" t="s">
+      <c r="E18" s="74" t="s">
         <v>54</v>
       </c>
-      <c r="F18" s="37" t="s">
+      <c r="F18" s="72" t="s">
         <v>91</v>
       </c>
-      <c r="G18" s="74" t="s">
+      <c r="G18" s="48" t="s">
         <v>92</v>
       </c>
-      <c r="H18" s="82" t="s">
+      <c r="H18" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="I18" s="83" t="s">
+      <c r="I18" s="25" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="19" spans="2:9" ht="85" x14ac:dyDescent="0.2">
-      <c r="B19" s="56"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="44" t="s">
+      <c r="B19" s="70"/>
+      <c r="C19" s="72"/>
+      <c r="D19" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="E19" s="55"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="74" t="s">
+      <c r="E19" s="74"/>
+      <c r="F19" s="72"/>
+      <c r="G19" s="48" t="s">
         <v>83</v>
       </c>
-      <c r="H19" s="37" t="s">
+      <c r="H19" s="72" t="s">
         <v>96</v>
       </c>
-      <c r="I19" s="37" t="s">
+      <c r="I19" s="72" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="20" spans="2:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="B20" s="56"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="84" t="s">
+      <c r="B20" s="70"/>
+      <c r="C20" s="72"/>
+      <c r="D20" s="56" t="s">
         <v>98</v>
       </c>
-      <c r="E20" s="55"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="74" t="s">
+      <c r="E20" s="74"/>
+      <c r="F20" s="72"/>
+      <c r="G20" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="H20" s="37"/>
-      <c r="I20" s="37"/>
+      <c r="H20" s="72"/>
+      <c r="I20" s="72"/>
     </row>
     <row r="21" spans="2:9" ht="86" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="85"/>
-      <c r="C21" s="86"/>
-      <c r="D21" s="87" t="s">
+      <c r="B21" s="71"/>
+      <c r="C21" s="73"/>
+      <c r="D21" s="57" t="s">
         <v>99</v>
       </c>
-      <c r="E21" s="88"/>
-      <c r="F21" s="86"/>
-      <c r="G21" s="89" t="s">
+      <c r="E21" s="75"/>
+      <c r="F21" s="73"/>
+      <c r="G21" s="58" t="s">
         <v>100</v>
       </c>
-      <c r="H21" s="86"/>
-      <c r="I21" s="86"/>
+      <c r="H21" s="73"/>
+      <c r="I21" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="E18:E21"/>
-    <mergeCell ref="F18:F21"/>
-    <mergeCell ref="H19:H21"/>
+    <mergeCell ref="I2:I6"/>
+    <mergeCell ref="G3:G6"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="C2:C6"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="E2:E6"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E11"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="F10:F11"/>
     <mergeCell ref="I19:I21"/>
     <mergeCell ref="B13:B16"/>
     <mergeCell ref="C13:C16"/>
@@ -2275,21 +2285,11 @@
     <mergeCell ref="I14:I16"/>
     <mergeCell ref="G15:G16"/>
     <mergeCell ref="H15:H16"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E11"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B2:B6"/>
-    <mergeCell ref="C2:C6"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="E2:E6"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="I2:I6"/>
-    <mergeCell ref="G3:G6"/>
-    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="E18:E21"/>
+    <mergeCell ref="F18:F21"/>
+    <mergeCell ref="H19:H21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>